<commit_message>
[Doc] Gantt Planning last version with use cases
</commit_message>
<xml_diff>
--- a/doc/Planning_Gantt.xlsx
+++ b/doc/Planning_Gantt.xlsx
@@ -12,9 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="694"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Prediction" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Task Name</t>
   </si>
@@ -86,25 +86,93 @@
     <t>These cells require manual input so the calculated cells have data to work with.</t>
   </si>
   <si>
-    <t>Débuggage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Configuration du module LoRa </t>
-  </si>
-  <si>
     <t>Montage SmartCanton DevBox</t>
   </si>
   <si>
-    <t>Configuration du module Bluetooth</t>
-  </si>
-  <si>
-    <t>Test du LoRa avec la DGSI</t>
-  </si>
-  <si>
     <t>Test avec les cartes de développement (LoRa + BLE)</t>
   </si>
   <si>
     <t>Tests des sensors de la carte</t>
+  </si>
+  <si>
+    <t>Test du LoRa avec le réseau DGSI</t>
+  </si>
+  <si>
+    <t>Débuggage carte électronique</t>
+  </si>
+  <si>
+    <t>Documentation des use cases</t>
+  </si>
+  <si>
+    <t>Etude et documentation de sécurité du Bluetooth</t>
+  </si>
+  <si>
+    <t>Mise en place de librairies pour la communication avec
+les différents périphériques</t>
+  </si>
+  <si>
+    <t>Documentation globale du projet</t>
+  </si>
+  <si>
+    <t>Relecture et correction du rapport</t>
+  </si>
+  <si>
+    <t>Analyse d'une API de communication entre les
+deux microcontrôleur (LoRa &lt;-&gt; BLE)</t>
+  </si>
+  <si>
+    <t>Use case déployement APPKEY : App android</t>
+  </si>
+  <si>
+    <t>Use case tracking GPS : Programmation KW41z</t>
+  </si>
+  <si>
+    <t>Use case tracking GPS : Application de visualisation</t>
+  </si>
+  <si>
+    <t>Use case scanner Bluetooth  : Programmation KW41z</t>
+  </si>
+  <si>
+    <t>Use case scanner Bluetooth  : Programmation LoRa</t>
+  </si>
+  <si>
+    <t>Use case tracking GPS : Programmation LoRa</t>
+  </si>
+  <si>
+    <t>Use case scanner Bluetooth  : Application de visualisation</t>
+  </si>
+  <si>
+    <t>Use case all sensors :  Programmation KW41z</t>
+  </si>
+  <si>
+    <t>Use case all sensors :  Programmation LoRa</t>
+  </si>
+  <si>
+    <t>Use case all sensors :  Application de visualisation</t>
+  </si>
+  <si>
+    <t>Programmation de l'API de communication 
+entre microcontrôleurs</t>
+  </si>
+  <si>
+    <t>Use case scanner Bluetooth  : Analyse sur l'implémentation</t>
+  </si>
+  <si>
+    <t>Use case déployement APPKEY : 
+Programmation KW41z + LoRa</t>
+  </si>
+  <si>
+    <t>Documentation en profondeur du projet</t>
+  </si>
+  <si>
+    <t>Use case all sensors : Analyse sur l'implémentation</t>
+  </si>
+  <si>
+    <t>Use case déployement APPKEY Bluetooth :
+Analyse sur l'implémentation</t>
+  </si>
+  <si>
+    <t>Use case tracking GPS : Analyse sur l'implémentation</t>
   </si>
 </sst>
 </file>
@@ -234,7 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -263,15 +331,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -280,6 +342,9 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -336,7 +401,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Prediction!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -355,9 +420,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$27</c:f>
+              <c:f>Prediction!$B$2:$B$36</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>Etat de l'art</c:v>
                 </c:pt>
@@ -383,29 +448,97 @@
                   <c:v>Montage SmartCanton DevBox</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Débuggage</c:v>
+                  <c:v>Débuggage carte électronique</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Configuration du module LoRa </c:v>
+                  <c:v>Tests des sensors de la carte</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Configuration du module Bluetooth</c:v>
+                  <c:v>Documentation des use cases</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Test du LoRa avec la DGSI</c:v>
+                  <c:v>Test du LoRa avec le réseau DGSI</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Tests des sensors de la carte</c:v>
+                  <c:v>Etude et documentation de sécurité du Bluetooth</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Analyse d'une API de communication entre les
+deux microcontrôleur (LoRa &lt;-&gt; BLE)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Programmation de l'API de communication 
+entre microcontrôleurs</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Mise en place de librairies pour la communication avec
+les différents périphériques</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Use case déployement APPKEY Bluetooth :
+Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Use case déployement APPKEY : 
+Programmation KW41z + LoRa</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Use case déployement APPKEY : App android</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Use case tracking GPS : Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Use case tracking GPS : Programmation KW41z</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Use case tracking GPS : Programmation LoRa</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Use case tracking GPS : Application de visualisation</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Use case scanner Bluetooth  : Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Use case scanner Bluetooth  : Programmation KW41z</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Use case scanner Bluetooth  : Programmation LoRa</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Use case scanner Bluetooth  : Application de visualisation</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Use case all sensors : Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Use case all sensors :  Programmation KW41z</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Use case all sensors :  Programmation LoRa</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Use case all sensors :  Application de visualisation</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Documentation globale du projet</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Documentation en profondeur du projet</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Relecture et correction du rapport</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$27</c:f>
+              <c:f>Prediction!$C$2:$C$36</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>42979</c:v>
                 </c:pt>
@@ -437,13 +570,76 @@
                   <c:v>43023</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43023</c:v>
+                  <c:v>43026</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>43026</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43030</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>43033</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>43033</c:v>
+                <c:pt idx="14">
+                  <c:v>43038</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43038</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43049</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43054</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43070</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43080</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43081</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43082</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43083</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43086</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43088</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43091</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43095</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43103</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43105</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43110</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43111</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>42979</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43101</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>42765</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -459,7 +655,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>Prediction!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -783,7 +979,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="16"/>
+            <c:idx val="20"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -797,15 +993,15 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000022-D5F0-426E-8956-F2E0AE099BB1}"/>
+                <c16:uniqueId val="{00000021-A4E4-4A89-89B6-B1CB6C8089AD}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$27</c:f>
+              <c:f>Prediction!$B$2:$B$36</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>Etat de l'art</c:v>
                 </c:pt>
@@ -831,34 +1027,102 @@
                   <c:v>Montage SmartCanton DevBox</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Débuggage</c:v>
+                  <c:v>Débuggage carte électronique</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Configuration du module LoRa </c:v>
+                  <c:v>Tests des sensors de la carte</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Configuration du module Bluetooth</c:v>
+                  <c:v>Documentation des use cases</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Test du LoRa avec la DGSI</c:v>
+                  <c:v>Test du LoRa avec le réseau DGSI</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Tests des sensors de la carte</c:v>
+                  <c:v>Etude et documentation de sécurité du Bluetooth</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Analyse d'une API de communication entre les
+deux microcontrôleur (LoRa &lt;-&gt; BLE)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Programmation de l'API de communication 
+entre microcontrôleurs</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Mise en place de librairies pour la communication avec
+les différents périphériques</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Use case déployement APPKEY Bluetooth :
+Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Use case déployement APPKEY : 
+Programmation KW41z + LoRa</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Use case déployement APPKEY : App android</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Use case tracking GPS : Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Use case tracking GPS : Programmation KW41z</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Use case tracking GPS : Programmation LoRa</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Use case tracking GPS : Application de visualisation</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Use case scanner Bluetooth  : Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Use case scanner Bluetooth  : Programmation KW41z</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Use case scanner Bluetooth  : Programmation LoRa</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Use case scanner Bluetooth  : Application de visualisation</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Use case all sensors : Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Use case all sensors :  Programmation KW41z</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Use case all sensors :  Programmation LoRa</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Use case all sensors :  Application de visualisation</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Documentation globale du projet</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Documentation en profondeur du projet</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Relecture et correction du rapport</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$27</c:f>
+              <c:f>Prediction!$F$2:$F$36</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>2.4000000000000004</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>10</c:v>
@@ -870,28 +1134,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -930,6 +1194,33 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -946,7 +1237,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>Prediction!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1270,7 +1561,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="16"/>
+            <c:idx val="20"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1284,15 +1575,15 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000045-D5F0-426E-8956-F2E0AE099BB1}"/>
+                <c16:uniqueId val="{00000043-A4E4-4A89-89B6-B1CB6C8089AD}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$27</c:f>
+              <c:f>Prediction!$B$2:$B$36</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>Etat de l'art</c:v>
                 </c:pt>
@@ -1318,31 +1609,99 @@
                   <c:v>Montage SmartCanton DevBox</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Débuggage</c:v>
+                  <c:v>Débuggage carte électronique</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Configuration du module LoRa </c:v>
+                  <c:v>Tests des sensors de la carte</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Configuration du module Bluetooth</c:v>
+                  <c:v>Documentation des use cases</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Test du LoRa avec la DGSI</c:v>
+                  <c:v>Test du LoRa avec le réseau DGSI</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Tests des sensors de la carte</c:v>
+                  <c:v>Etude et documentation de sécurité du Bluetooth</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Analyse d'une API de communication entre les
+deux microcontrôleur (LoRa &lt;-&gt; BLE)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Programmation de l'API de communication 
+entre microcontrôleurs</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Mise en place de librairies pour la communication avec
+les différents périphériques</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Use case déployement APPKEY Bluetooth :
+Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Use case déployement APPKEY : 
+Programmation KW41z + LoRa</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Use case déployement APPKEY : App android</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Use case tracking GPS : Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Use case tracking GPS : Programmation KW41z</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Use case tracking GPS : Programmation LoRa</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Use case tracking GPS : Application de visualisation</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Use case scanner Bluetooth  : Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Use case scanner Bluetooth  : Programmation KW41z</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Use case scanner Bluetooth  : Programmation LoRa</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Use case scanner Bluetooth  : Application de visualisation</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Use case all sensors : Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Use case all sensors :  Programmation KW41z</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Use case all sensors :  Programmation LoRa</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Use case all sensors :  Application de visualisation</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Documentation globale du projet</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Documentation en profondeur du projet</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Relecture et correction du rapport</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$27</c:f>
+              <c:f>Prediction!$G$2:$G$36</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>0.59999999999999964</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1357,66 +1716,93 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.6</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="14">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="24">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="26">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="27">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>142.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="34">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2151,8 +2537,8 @@
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2479,19 +2865,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S51"/>
+  <dimension ref="B1:S60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="46.7109375" customWidth="1"/>
+    <col min="2" max="2" width="52.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="8" width="14.42578125" customWidth="1"/>
     <col min="9" max="9" width="4" customWidth="1"/>
     <col min="10" max="10" width="28.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
     <col min="12" max="12" width="2.28515625" customWidth="1"/>
     <col min="13" max="13" width="12.42578125" customWidth="1"/>
     <col min="18" max="18" width="20.140625" customWidth="1"/>
@@ -2530,17 +2917,17 @@
         <f>C2</f>
         <v>42979</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-    </row>
-    <row r="2" spans="2:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+    </row>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
@@ -2548,25 +2935,25 @@
         <v>42979</v>
       </c>
       <c r="D2" s="7">
-        <f t="shared" ref="D2:D27" si="0">IF(ISBLANK(E2),"",E2+C2)</f>
-        <v>42982</v>
+        <f t="shared" ref="D2:D36" si="0">IF(ISBLANK(E2),"",E2+C2)</f>
+        <v>42989</v>
       </c>
       <c r="E2" s="8">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F2" s="9">
         <f t="shared" ref="F2:F11" si="1">IF(((D2)=""),"",(H2)*(D2-C2))</f>
-        <v>2.4000000000000004</v>
+        <v>8</v>
       </c>
       <c r="G2" s="9">
         <f t="shared" ref="G2:G11" si="2">IF(F2="","",(D2-C2)-F2)</f>
-        <v>0.59999999999999964</v>
+        <v>2</v>
       </c>
       <c r="H2" s="10">
         <v>0.8</v>
       </c>
     </row>
-    <row r="3" spans="2:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
@@ -2575,14 +2962,14 @@
       </c>
       <c r="D3" s="7">
         <f t="shared" si="0"/>
-        <v>42984</v>
+        <v>42987</v>
       </c>
       <c r="E3" s="11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F3" s="9">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G3" s="9">
         <f t="shared" si="2"/>
@@ -2593,7 +2980,7 @@
       </c>
       <c r="J3" s="12"/>
     </row>
-    <row r="4" spans="2:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
@@ -2620,7 +3007,7 @@
       </c>
       <c r="J4" s="12"/>
     </row>
-    <row r="5" spans="2:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
@@ -2646,7 +3033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
@@ -2672,9 +3059,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C7" s="6">
         <v>42998</v>
@@ -2688,17 +3075,17 @@
       </c>
       <c r="F7" s="9">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G7" s="9">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H7" s="10">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
@@ -2714,19 +3101,19 @@
       </c>
       <c r="F8" s="9">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>2</v>
       </c>
       <c r="G8" s="9">
         <f t="shared" si="2"/>
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="H8" s="10">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" s="6">
         <v>43018</v>
@@ -2740,45 +3127,45 @@
       </c>
       <c r="F9" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G9" s="9">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H9" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C10" s="6">
         <v>43020</v>
       </c>
       <c r="D10" s="7">
         <f t="shared" si="0"/>
-        <v>43023</v>
+        <v>43025</v>
       </c>
       <c r="E10" s="11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F10" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G10" s="9">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H10" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="6">
         <v>43023</v>
@@ -2792,605 +3179,911 @@
       </c>
       <c r="F11" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G11" s="9">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H11" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C12" s="6">
-        <v>43023</v>
+        <v>43026</v>
       </c>
       <c r="D12" s="7">
         <f t="shared" si="0"/>
-        <v>43033</v>
+        <v>43028</v>
       </c>
       <c r="E12" s="11">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F12" s="9">
-        <f t="shared" ref="F12:F27" si="3">IF(((D12)=""),"",(H12)*(D12-C12))</f>
-        <v>0</v>
+        <f t="shared" ref="F12:F36" si="3">IF(((D12)=""),"",(H12)*(D12-C12))</f>
+        <v>2</v>
       </c>
       <c r="G12" s="9">
-        <f t="shared" ref="G12:G27" si="4">IF(F12="","",(D12-C12)-F12)</f>
-        <v>10</v>
+        <f t="shared" ref="G12:G36" si="4">IF(F12="","",(D12-C12)-F12)</f>
+        <v>0</v>
       </c>
       <c r="H12" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="6">
-        <v>43033</v>
+        <v>43026</v>
       </c>
       <c r="D13" s="7">
         <f t="shared" si="0"/>
-        <v>43053</v>
+        <v>43029</v>
       </c>
       <c r="E13" s="11">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F13" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G13" s="9">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="H13" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="6">
-        <v>43033</v>
+        <v>43030</v>
       </c>
       <c r="D14" s="7">
         <f t="shared" si="0"/>
-        <v>43053</v>
+        <v>43040</v>
       </c>
       <c r="E14" s="11">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F14" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="9">
         <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="6">
+        <v>43033</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="0"/>
+        <v>43043</v>
+      </c>
+      <c r="E15" s="11">
+        <v>10</v>
+      </c>
+      <c r="F15" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="9">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="H15" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="6">
+        <v>43038</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" si="0"/>
+        <v>43048</v>
+      </c>
+      <c r="E16" s="11">
+        <v>10</v>
+      </c>
+      <c r="F16" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="9">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="H16" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="6">
+        <v>43038</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="0"/>
+        <v>43068</v>
+      </c>
+      <c r="E17" s="11">
+        <v>30</v>
+      </c>
+      <c r="F17" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="9">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="H17" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="6">
+        <v>43049</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" si="0"/>
+        <v>43054</v>
+      </c>
+      <c r="E18" s="11">
+        <v>5</v>
+      </c>
+      <c r="F18" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="9">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="6">
+        <v>43054</v>
+      </c>
+      <c r="D19" s="7">
+        <f t="shared" si="0"/>
+        <v>43074</v>
+      </c>
+      <c r="E19" s="11">
         <v>20</v>
       </c>
-      <c r="H14" s="10">
-        <v>0</v>
-      </c>
-      <c r="J14" s="13"/>
-    </row>
-    <row r="15" spans="2:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7" t="str">
+      <c r="F19" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="9">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="H19" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="6">
+        <v>43070</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="0"/>
+        <v>43080</v>
+      </c>
+      <c r="E20" s="11">
+        <v>10</v>
+      </c>
+      <c r="F20" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="9">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="6">
+        <v>43080</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="0"/>
+        <v>43081</v>
+      </c>
+      <c r="E21" s="11">
+        <v>1</v>
+      </c>
+      <c r="F21" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="9">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="H21" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="6">
+        <v>43081</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="0"/>
+        <v>43084</v>
+      </c>
+      <c r="E22" s="11">
+        <v>3</v>
+      </c>
+      <c r="F22" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="9">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="H22" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="6">
+        <v>43082</v>
+      </c>
+      <c r="D23" s="7">
+        <f t="shared" si="0"/>
+        <v>43085</v>
+      </c>
+      <c r="E23" s="15">
+        <v>3</v>
+      </c>
+      <c r="F23" s="9">
+        <f t="shared" ref="F23" si="5">IF(((D23)=""),"",(H23)*(D23-C23))</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="9">
+        <f t="shared" ref="G23" si="6">IF(F23="","",(D23-C23)-F23)</f>
+        <v>3</v>
+      </c>
+      <c r="H23" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="6">
+        <v>43083</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" si="0"/>
+        <v>43086</v>
+      </c>
+      <c r="E24" s="15">
+        <v>3</v>
+      </c>
+      <c r="F24" s="9">
+        <f t="shared" ref="F24:F25" si="7">IF(((D24)=""),"",(H24)*(D24-C24))</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="9">
+        <f t="shared" ref="G24:G25" si="8">IF(F24="","",(D24-C24)-F24)</f>
+        <v>3</v>
+      </c>
+      <c r="H24" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="14">
+        <v>43086</v>
+      </c>
+      <c r="D25" s="7">
+        <f t="shared" si="0"/>
+        <v>43088</v>
+      </c>
+      <c r="E25" s="15">
+        <v>2</v>
+      </c>
+      <c r="F25" s="9">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="9">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="H25" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="14">
+        <v>43088</v>
+      </c>
+      <c r="D26" s="7">
+        <f t="shared" si="0"/>
+        <v>43093</v>
+      </c>
+      <c r="E26" s="15">
+        <v>5</v>
+      </c>
+      <c r="F26" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="9">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="H26" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="14">
+        <v>43091</v>
+      </c>
+      <c r="D27" s="7">
+        <f t="shared" si="0"/>
+        <v>43094</v>
+      </c>
+      <c r="E27" s="11">
+        <v>3</v>
+      </c>
+      <c r="F27" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="9">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="H27" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="14">
+        <v>43095</v>
+      </c>
+      <c r="D28" s="7">
+        <f t="shared" si="0"/>
+        <v>43105</v>
+      </c>
+      <c r="E28" s="11">
+        <v>10</v>
+      </c>
+      <c r="F28" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G28" s="9">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="H28" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="6">
+        <v>43103</v>
+      </c>
+      <c r="D29" s="7">
+        <f t="shared" si="0"/>
+        <v>43105</v>
+      </c>
+      <c r="E29" s="11">
+        <v>2</v>
+      </c>
+      <c r="F29" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="9">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="H29" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="6">
+        <v>43105</v>
+      </c>
+      <c r="D30" s="7">
+        <f t="shared" si="0"/>
+        <v>43110</v>
+      </c>
+      <c r="E30" s="11">
+        <v>5</v>
+      </c>
+      <c r="F30" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="9">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="H30" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="6">
+        <v>43110</v>
+      </c>
+      <c r="D31" s="7">
+        <f t="shared" ref="D31:D32" si="9">IF(ISBLANK(E31),"",E31+C31)</f>
+        <v>43111</v>
+      </c>
+      <c r="E31" s="11">
+        <v>1</v>
+      </c>
+      <c r="F31" s="9">
+        <f t="shared" ref="F31:F32" si="10">IF(((D31)=""),"",(H31)*(D31-C31))</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="9">
+        <f t="shared" ref="G31:G32" si="11">IF(F31="","",(D31-C31)-F31)</f>
+        <v>1</v>
+      </c>
+      <c r="H31" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="6">
+        <v>43111</v>
+      </c>
+      <c r="D32" s="7">
+        <f t="shared" si="9"/>
+        <v>43114</v>
+      </c>
+      <c r="E32" s="11">
+        <v>3</v>
+      </c>
+      <c r="F32" s="9">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="9">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="H32" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="6">
+        <v>42979</v>
+      </c>
+      <c r="D33" s="7">
+        <f t="shared" si="0"/>
+        <v>43129</v>
+      </c>
+      <c r="E33" s="11">
+        <v>150</v>
+      </c>
+      <c r="F33" s="9">
+        <f t="shared" si="3"/>
+        <v>7.5</v>
+      </c>
+      <c r="G33" s="9">
+        <f t="shared" si="4"/>
+        <v>142.5</v>
+      </c>
+      <c r="H33" s="10">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="34" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="6">
+        <v>43101</v>
+      </c>
+      <c r="D34" s="7">
+        <f t="shared" si="0"/>
+        <v>43131</v>
+      </c>
+      <c r="E34" s="11">
+        <v>30</v>
+      </c>
+      <c r="F34" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G34" s="9">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="H34" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="6">
+        <v>42765</v>
+      </c>
+      <c r="D35" s="7">
+        <f t="shared" si="0"/>
+        <v>42775</v>
+      </c>
+      <c r="E35" s="11">
+        <v>10</v>
+      </c>
+      <c r="F35" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G35" s="9">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="H35" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="5"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="7" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="9" t="str">
+      <c r="E36" s="11"/>
+      <c r="F36" s="9" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="G15" s="9" t="str">
+      <c r="G36" s="9" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="H15" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G16" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H16" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G17" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H17" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G18" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H18" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G19" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H19" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="18"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G20" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H20" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G21" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H21" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G22" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H22" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G23" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H23" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G24" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H24" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G25" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H25" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G26" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H26" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="5"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G27" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H27" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="19"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="12"/>
-    </row>
-    <row r="29" spans="2:18" ht="21" x14ac:dyDescent="0.25">
-      <c r="B29" s="19"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="12"/>
-      <c r="J29" s="21" t="s">
+      <c r="H36" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="17"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="12"/>
+    </row>
+    <row r="38" spans="2:18" ht="21" x14ac:dyDescent="0.25">
+      <c r="B38" s="17"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="12"/>
+      <c r="J38" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="K29" s="24" t="s">
+      <c r="K38" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="24"/>
-      <c r="O29" s="24"/>
-      <c r="P29" s="25" t="s">
+      <c r="L38" s="23"/>
+      <c r="M38" s="23"/>
+      <c r="N38" s="23"/>
+      <c r="O38" s="23"/>
+      <c r="P38" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="25"/>
-      <c r="R29" s="25"/>
-    </row>
-    <row r="30" spans="2:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="19"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="K30" s="26" t="s">
+      <c r="Q38" s="24"/>
+      <c r="R38" s="24"/>
+    </row>
+    <row r="39" spans="2:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="17"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="K39" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="L30" s="26"/>
-      <c r="M30" s="26"/>
-      <c r="N30" s="26"/>
-      <c r="O30" s="26"/>
-      <c r="P30" s="26" t="s">
+      <c r="L39" s="25"/>
+      <c r="M39" s="25"/>
+      <c r="N39" s="25"/>
+      <c r="O39" s="25"/>
+      <c r="P39" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="Q30" s="26"/>
-      <c r="R30" s="26"/>
-    </row>
-    <row r="31" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="19"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-    </row>
-    <row r="32" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="19"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-    </row>
-    <row r="33" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="19"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-    </row>
-    <row r="34" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="19"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-    </row>
-    <row r="35" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="19"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-    </row>
-    <row r="36" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="19"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-    </row>
-    <row r="37" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="19"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-    </row>
-    <row r="38" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="19"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-    </row>
-    <row r="39" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="19"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-    </row>
-    <row r="40" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="19"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-    </row>
-    <row r="41" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="19"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-    </row>
-    <row r="42" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="19"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-    </row>
-    <row r="43" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="19"/>
+      <c r="Q39" s="25"/>
+      <c r="R39" s="25"/>
+    </row>
+    <row r="40" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="17"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+    </row>
+    <row r="41" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="17"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+    </row>
+    <row r="42" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="17"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+    </row>
+    <row r="43" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="17"/>
       <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-    </row>
-    <row r="44" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="19"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-    </row>
-    <row r="45" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="19"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-    </row>
-    <row r="46" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="19"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
-    </row>
-    <row r="47" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="19"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-    </row>
-    <row r="48" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="19"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="20"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+    </row>
+    <row r="44" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="17"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+    </row>
+    <row r="45" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="17"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+    </row>
+    <row r="46" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="17"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+    </row>
+    <row r="47" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="17"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+    </row>
+    <row r="48" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="17"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
     </row>
     <row r="49" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="19"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
     </row>
     <row r="50" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="19"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
     </row>
     <row r="51" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="19"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+    </row>
+    <row r="52" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="17"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+    </row>
+    <row r="53" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="17"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+    </row>
+    <row r="54" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="17"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+    </row>
+    <row r="55" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="17"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+    </row>
+    <row r="56" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="17"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+    </row>
+    <row r="57" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="17"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+    </row>
+    <row r="58" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="17"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18"/>
+    </row>
+    <row r="59" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="17"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
+    </row>
+    <row r="60" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="17"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="M1:S1"/>
-    <mergeCell ref="K29:O29"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="K30:O30"/>
-    <mergeCell ref="P30:R30"/>
+    <mergeCell ref="K38:O38"/>
+    <mergeCell ref="P38:R38"/>
+    <mergeCell ref="K39:O39"/>
+    <mergeCell ref="P39:R39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
[Doc] Gantt Planning update
</commit_message>
<xml_diff>
--- a/doc/Planning_Gantt.xlsx
+++ b/doc/Planning_Gantt.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Prediction" sheetId="1" r:id="rId1"/>
+    <sheet name="Real" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="49">
   <si>
     <t>Task Name</t>
   </si>
@@ -158,21 +159,25 @@
     <t>Use case scanner Bluetooth  : Analyse sur l'implémentation</t>
   </si>
   <si>
-    <t>Use case déployement APPKEY : 
-Programmation KW41z + LoRa</t>
-  </si>
-  <si>
     <t>Documentation en profondeur du projet</t>
   </si>
   <si>
     <t>Use case all sensors : Analyse sur l'implémentation</t>
   </si>
   <si>
-    <t>Use case déployement APPKEY Bluetooth :
+    <t>Use case tracking GPS : Analyse sur l'implémentation</t>
+  </si>
+  <si>
+    <t>Use case deployment APPKEY Bluetooth :
 Analyse sur l'implémentation</t>
   </si>
   <si>
-    <t>Use case tracking GPS : Analyse sur l'implémentation</t>
+    <t>Use case deployment APPKEY : 
+Programmation KW41z + LoRa</t>
+  </si>
+  <si>
+    <t>Use case deployment APPKEY : 
+Programmation serveur REST de partage de clés</t>
   </si>
 </sst>
 </file>
@@ -422,7 +427,7 @@
             <c:strRef>
               <c:f>Prediction!$B$2:$B$36</c:f>
               <c:strCache>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>Etat de l'art</c:v>
                 </c:pt>
@@ -475,59 +480,63 @@
 les différents périphériques</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Use case déployement APPKEY Bluetooth :
+                  <c:v>Use case deployment APPKEY Bluetooth :
 Analyse sur l'implémentation</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Use case déployement APPKEY : 
+                  <c:v>Use case deployment APPKEY : 
 Programmation KW41z + LoRa</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>Use case deployment APPKEY : 
+Programmation serveur REST de partage de clés</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Use case déployement APPKEY : App android</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>Use case tracking GPS : Analyse sur l'implémentation</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>Use case tracking GPS : Programmation KW41z</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>Use case tracking GPS : Programmation LoRa</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>Use case tracking GPS : Application de visualisation</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>Use case scanner Bluetooth  : Analyse sur l'implémentation</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>Use case scanner Bluetooth  : Programmation KW41z</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>Use case scanner Bluetooth  : Programmation LoRa</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>Use case scanner Bluetooth  : Application de visualisation</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>Use case all sensors : Analyse sur l'implémentation</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>Use case all sensors :  Programmation KW41z</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>Use case all sensors :  Programmation LoRa</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>Use case all sensors :  Application de visualisation</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>Documentation globale du projet</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>Documentation en profondeur du projet</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>Relecture et correction du rapport</c:v>
                 </c:pt>
               </c:strCache>
@@ -597,48 +606,51 @@
                   <c:v>43070</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>43070</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>43080</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>43081</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>43082</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>43083</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>43086</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>43088</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>43091</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>43095</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>43103</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>43105</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>43110</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>43111</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>42979</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>43101</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>42765</c:v>
                 </c:pt>
               </c:numCache>
@@ -1001,7 +1013,7 @@
             <c:strRef>
               <c:f>Prediction!$B$2:$B$36</c:f>
               <c:strCache>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>Etat de l'art</c:v>
                 </c:pt>
@@ -1054,59 +1066,63 @@
 les différents périphériques</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Use case déployement APPKEY Bluetooth :
+                  <c:v>Use case deployment APPKEY Bluetooth :
 Analyse sur l'implémentation</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Use case déployement APPKEY : 
+                  <c:v>Use case deployment APPKEY : 
 Programmation KW41z + LoRa</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>Use case deployment APPKEY : 
+Programmation serveur REST de partage de clés</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Use case déployement APPKEY : App android</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>Use case tracking GPS : Analyse sur l'implémentation</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>Use case tracking GPS : Programmation KW41z</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>Use case tracking GPS : Programmation LoRa</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>Use case tracking GPS : Application de visualisation</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>Use case scanner Bluetooth  : Analyse sur l'implémentation</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>Use case scanner Bluetooth  : Programmation KW41z</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>Use case scanner Bluetooth  : Programmation LoRa</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>Use case scanner Bluetooth  : Application de visualisation</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>Use case all sensors : Analyse sur l'implémentation</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>Use case all sensors :  Programmation KW41z</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>Use case all sensors :  Programmation LoRa</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>Use case all sensors :  Application de visualisation</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>Documentation globale du projet</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>Documentation en profondeur du projet</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>Relecture et correction du rapport</c:v>
                 </c:pt>
               </c:strCache>
@@ -1212,10 +1228,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>0</c:v>
@@ -1583,7 +1599,7 @@
             <c:strRef>
               <c:f>Prediction!$B$2:$B$36</c:f>
               <c:strCache>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>Etat de l'art</c:v>
                 </c:pt>
@@ -1636,59 +1652,63 @@
 les différents périphériques</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Use case déployement APPKEY Bluetooth :
+                  <c:v>Use case deployment APPKEY Bluetooth :
 Analyse sur l'implémentation</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Use case déployement APPKEY : 
+                  <c:v>Use case deployment APPKEY : 
 Programmation KW41z + LoRa</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>Use case deployment APPKEY : 
+Programmation serveur REST de partage de clés</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Use case déployement APPKEY : App android</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>Use case tracking GPS : Analyse sur l'implémentation</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>Use case tracking GPS : Programmation KW41z</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>Use case tracking GPS : Programmation LoRa</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>Use case tracking GPS : Application de visualisation</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>Use case scanner Bluetooth  : Analyse sur l'implémentation</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>Use case scanner Bluetooth  : Programmation KW41z</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>Use case scanner Bluetooth  : Programmation LoRa</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>Use case scanner Bluetooth  : Application de visualisation</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>Use case all sensors : Analyse sur l'implémentation</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>Use case all sensors :  Programmation KW41z</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>Use case all sensors :  Programmation LoRa</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>Use case all sensors :  Application de visualisation</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>Documentation globale du projet</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>Documentation en profondeur du projet</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>Relecture et correction du rapport</c:v>
                 </c:pt>
               </c:strCache>
@@ -1740,7 +1760,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>10</c:v>
@@ -1758,10 +1778,10 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>3</c:v>
@@ -1770,40 +1790,40 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="23">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>142.5</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1811,6 +1831,1622 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000046-D5F0-426E-8956-F2E0AE099BB1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="-2095074752"/>
+        <c:axId val="-2095144704"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2095074752"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2095144704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2095144704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="42979"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2095074752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="0"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Real!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Start Date</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Real!$B$2:$B$37</c:f>
+              <c:strCache>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>Etat de l'art</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Choix des composants et comparatifs</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Réalisation de la schématique du circuit </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Routage du circuit</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Check DRC du circuit</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Test avec les cartes de développement (LoRa + BLE)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Liste du matériel à commander</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Montage SmartCanton DevBox</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Débuggage carte électronique</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Tests des sensors de la carte</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Documentation des use cases</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Test du LoRa avec le réseau DGSI</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Etude et documentation de sécurité du Bluetooth</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Analyse d'une API de communication entre les
+deux microcontrôleur (LoRa &lt;-&gt; BLE)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Programmation de l'API de communication 
+entre microcontrôleurs</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Mise en place de librairies pour la communication avec
+les différents périphériques</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Use case deployment APPKEY Bluetooth :
+Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Use case deployment APPKEY : 
+Programmation KW41z + LoRa</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Use case deployment APPKEY : 
+Programmation serveur REST de partage de clés</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Use case déployement APPKEY : App android</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Use case tracking GPS : Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Use case tracking GPS : Programmation KW41z</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Use case tracking GPS : Programmation LoRa</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Use case tracking GPS : Application de visualisation</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Use case scanner Bluetooth  : Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Use case scanner Bluetooth  : Programmation KW41z</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Use case scanner Bluetooth  : Programmation LoRa</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Use case scanner Bluetooth  : Application de visualisation</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Use case all sensors : Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Use case all sensors :  Programmation KW41z</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Use case all sensors :  Programmation LoRa</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Use case all sensors :  Application de visualisation</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Documentation globale du projet</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Documentation en profondeur du projet</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Relecture et correction du rapport</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Real!$C$2:$C$37</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>42979</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42982</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42982</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42992</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43018</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43020</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43023</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43026</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43026</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43030</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43033</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43038</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43038</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43049</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43054</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43070</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43070</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43080</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43081</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43082</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43083</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43086</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43088</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43091</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43095</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43103</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43105</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43110</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43111</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>42979</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43101</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>42765</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C368-4F52-A25D-40FC19E6C294}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Real!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Days Complete</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="72C9DE"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="72C9DE"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="528E77"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="528E77"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="528E77"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="B86FD7"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="B86FD7"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000E-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="B86FD7"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000010-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C14B3A"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000012-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C14B3A"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000014-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="72C9DE"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000016-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="72C9DE"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000018-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="72C9DE"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001A-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="528E77"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001C-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="528E77"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001E-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="B86FD7"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000020-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="21"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="B86FD7"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Real!$B$2:$B$37</c:f>
+              <c:strCache>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>Etat de l'art</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Choix des composants et comparatifs</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Réalisation de la schématique du circuit </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Routage du circuit</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Check DRC du circuit</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Test avec les cartes de développement (LoRa + BLE)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Liste du matériel à commander</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Montage SmartCanton DevBox</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Débuggage carte électronique</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Tests des sensors de la carte</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Documentation des use cases</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Test du LoRa avec le réseau DGSI</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Etude et documentation de sécurité du Bluetooth</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Analyse d'une API de communication entre les
+deux microcontrôleur (LoRa &lt;-&gt; BLE)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Programmation de l'API de communication 
+entre microcontrôleurs</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Mise en place de librairies pour la communication avec
+les différents périphériques</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Use case deployment APPKEY Bluetooth :
+Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Use case deployment APPKEY : 
+Programmation KW41z + LoRa</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Use case deployment APPKEY : 
+Programmation serveur REST de partage de clés</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Use case déployement APPKEY : App android</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Use case tracking GPS : Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Use case tracking GPS : Programmation KW41z</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Use case tracking GPS : Programmation LoRa</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Use case tracking GPS : Application de visualisation</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Use case scanner Bluetooth  : Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Use case scanner Bluetooth  : Programmation KW41z</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Use case scanner Bluetooth  : Programmation LoRa</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Use case scanner Bluetooth  : Application de visualisation</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Use case all sensors : Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Use case all sensors :  Programmation KW41z</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Use case all sensors :  Programmation LoRa</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Use case all sensors :  Application de visualisation</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Documentation globale du projet</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Documentation en profondeur du projet</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Relecture et correction du rapport</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Real!$F$2:$F$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000023-C368-4F52-A25D-40FC19E6C294}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Real!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Days Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="BBE6EF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000025-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="BBE6EF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000027-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="AFD3C5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000029-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="AFD3C5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002B-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="AFD3C5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002D-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="D5A8E7"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002F-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="D5A8E7"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000031-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="D5A8E7"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000033-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="E3B3AA"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000035-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="E3B3AA"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000037-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="BBE6EF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000039-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="BBE6EF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003B-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="BBE6EF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003D-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="AFD3C5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003F-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="AFD3C5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000041-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="D5A8E7"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000043-C368-4F52-A25D-40FC19E6C294}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="21"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="D5A8E7"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Real!$B$2:$B$37</c:f>
+              <c:strCache>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>Etat de l'art</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Choix des composants et comparatifs</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Réalisation de la schématique du circuit </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Routage du circuit</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Check DRC du circuit</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Test avec les cartes de développement (LoRa + BLE)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Liste du matériel à commander</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Montage SmartCanton DevBox</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Débuggage carte électronique</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Tests des sensors de la carte</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Documentation des use cases</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Test du LoRa avec le réseau DGSI</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Etude et documentation de sécurité du Bluetooth</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Analyse d'une API de communication entre les
+deux microcontrôleur (LoRa &lt;-&gt; BLE)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Programmation de l'API de communication 
+entre microcontrôleurs</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Mise en place de librairies pour la communication avec
+les différents périphériques</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Use case deployment APPKEY Bluetooth :
+Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Use case deployment APPKEY : 
+Programmation KW41z + LoRa</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Use case deployment APPKEY : 
+Programmation serveur REST de partage de clés</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Use case déployement APPKEY : App android</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Use case tracking GPS : Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Use case tracking GPS : Programmation KW41z</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Use case tracking GPS : Programmation LoRa</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Use case tracking GPS : Application de visualisation</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Use case scanner Bluetooth  : Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Use case scanner Bluetooth  : Programmation KW41z</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Use case scanner Bluetooth  : Programmation LoRa</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Use case scanner Bluetooth  : Application de visualisation</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Use case all sensors : Analyse sur l'implémentation</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Use case all sensors :  Programmation KW41z</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Use case all sensors :  Programmation LoRa</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Use case all sensors :  Application de visualisation</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Documentation globale du projet</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Documentation en profondeur du projet</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Relecture et correction du rapport</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Real!$G$2:$G$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>142.5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000046-C368-4F52-A25D-40FC19E6C294}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2020,7 +3656,552 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2568,6 +4749,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>253999</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5D701EE-A3CE-48AF-8565-B2C532585363}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2868,7 +5092,7 @@
   <dimension ref="B1:S60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2935,18 +5159,18 @@
         <v>42979</v>
       </c>
       <c r="D2" s="7">
-        <f t="shared" ref="D2:D36" si="0">IF(ISBLANK(E2),"",E2+C2)</f>
+        <f t="shared" ref="D2:D37" si="0">IF(ISBLANK(E2),"",E2+C2)</f>
         <v>42989</v>
       </c>
       <c r="E2" s="8">
         <v>10</v>
       </c>
       <c r="F2" s="9">
-        <f t="shared" ref="F2:F11" si="1">IF(((D2)=""),"",(H2)*(D2-C2))</f>
+        <f t="shared" ref="F2:F37" si="1">IF(((D2)=""),"",(H2)*(D2-C2))</f>
         <v>8</v>
       </c>
       <c r="G2" s="9">
-        <f t="shared" ref="G2:G11" si="2">IF(F2="","",(D2-C2)-F2)</f>
+        <f t="shared" ref="G2:G37" si="2">IF(F2="","",(D2-C2)-F2)</f>
         <v>2</v>
       </c>
       <c r="H2" s="10">
@@ -3204,11 +5428,11 @@
         <v>2</v>
       </c>
       <c r="F12" s="9">
-        <f t="shared" ref="F12:F36" si="3">IF(((D12)=""),"",(H12)*(D12-C12))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="G12" s="9">
-        <f t="shared" ref="G12:G36" si="4">IF(F12="","",(D12-C12)-F12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H12" s="10">
@@ -3230,11 +5454,11 @@
         <v>3</v>
       </c>
       <c r="F13" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="G13" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H13" s="10">
@@ -3256,11 +5480,11 @@
         <v>10</v>
       </c>
       <c r="F14" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G14" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="H14" s="10">
@@ -3277,18 +5501,18 @@
       </c>
       <c r="D15" s="7">
         <f t="shared" si="0"/>
-        <v>43043</v>
+        <v>43038</v>
       </c>
       <c r="E15" s="11">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F15" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G15" s="9">
-        <f t="shared" si="4"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="H15" s="10">
         <v>0</v>
@@ -3309,11 +5533,11 @@
         <v>10</v>
       </c>
       <c r="F16" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="H16" s="10">
@@ -3335,11 +5559,11 @@
         <v>30</v>
       </c>
       <c r="F17" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G17" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="H17" s="10">
@@ -3361,11 +5585,11 @@
         <v>5</v>
       </c>
       <c r="F18" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G18" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="H18" s="10">
@@ -3374,7 +5598,7 @@
     </row>
     <row r="19" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="21" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C19" s="6">
         <v>43054</v>
@@ -3387,20 +5611,20 @@
         <v>20</v>
       </c>
       <c r="F19" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G19" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="H19" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="21" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C20" s="6">
         <v>43070</v>
@@ -3413,11 +5637,11 @@
         <v>10</v>
       </c>
       <c r="F20" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G20" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="H20" s="10">
@@ -3426,51 +5650,51 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="21" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C21" s="6">
-        <v>43080</v>
+        <v>43070</v>
       </c>
       <c r="D21" s="7">
         <f t="shared" si="0"/>
-        <v>43081</v>
+        <v>43080</v>
       </c>
       <c r="E21" s="11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G21" s="9">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="H21" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>32</v>
+      <c r="B22" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="C22" s="6">
-        <v>43081</v>
+        <v>43080</v>
       </c>
       <c r="D22" s="7">
         <f t="shared" si="0"/>
-        <v>43084</v>
+        <v>43081</v>
       </c>
       <c r="E22" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F22" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G22" s="9">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="H22" s="10">
         <v>0</v>
@@ -3478,50 +5702,50 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C23" s="6">
-        <v>43082</v>
+        <v>43081</v>
       </c>
       <c r="D23" s="7">
         <f t="shared" si="0"/>
-        <v>43085</v>
-      </c>
-      <c r="E23" s="15">
+        <v>43084</v>
+      </c>
+      <c r="E23" s="11">
         <v>3</v>
       </c>
       <c r="F23" s="9">
-        <f t="shared" ref="F23" si="5">IF(((D23)=""),"",(H23)*(D23-C23))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G23" s="9">
-        <f t="shared" ref="G23" si="6">IF(F23="","",(D23-C23)-F23)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="H23" s="16">
+      <c r="H23" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C24" s="6">
-        <v>43083</v>
+        <v>43082</v>
       </c>
       <c r="D24" s="7">
         <f t="shared" si="0"/>
-        <v>43086</v>
+        <v>43085</v>
       </c>
       <c r="E24" s="15">
         <v>3</v>
       </c>
       <c r="F24" s="9">
-        <f t="shared" ref="F24:F25" si="7">IF(((D24)=""),"",(H24)*(D24-C24))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G24" s="9">
-        <f t="shared" ref="G24:G25" si="8">IF(F24="","",(D24-C24)-F24)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H24" s="16">
@@ -3530,25 +5754,25 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="14">
-        <v>43086</v>
+        <v>33</v>
+      </c>
+      <c r="C25" s="6">
+        <v>43083</v>
       </c>
       <c r="D25" s="7">
         <f t="shared" si="0"/>
-        <v>43088</v>
+        <v>43086</v>
       </c>
       <c r="E25" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F25" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G25" s="9">
-        <f t="shared" si="8"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="H25" s="16">
         <v>0</v>
@@ -3556,25 +5780,25 @@
     </row>
     <row r="26" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C26" s="14">
-        <v>43088</v>
+        <v>43086</v>
       </c>
       <c r="D26" s="7">
         <f t="shared" si="0"/>
-        <v>43093</v>
+        <v>43088</v>
       </c>
       <c r="E26" s="15">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F26" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G26" s="9">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="H26" s="16">
         <v>0</v>
@@ -3582,51 +5806,51 @@
     </row>
     <row r="27" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="14">
-        <v>43091</v>
+        <v>43088</v>
       </c>
       <c r="D27" s="7">
         <f t="shared" si="0"/>
-        <v>43094</v>
-      </c>
-      <c r="E27" s="11">
-        <v>3</v>
+        <v>43093</v>
+      </c>
+      <c r="E27" s="15">
+        <v>5</v>
       </c>
       <c r="F27" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G27" s="9">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="H27" s="10">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="H27" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C28" s="14">
-        <v>43095</v>
+        <v>43091</v>
       </c>
       <c r="D28" s="7">
         <f t="shared" si="0"/>
-        <v>43105</v>
+        <v>43094</v>
       </c>
       <c r="E28" s="11">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F28" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G28" s="9">
-        <f t="shared" si="4"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="H28" s="10">
         <v>0</v>
@@ -3634,25 +5858,25 @@
     </row>
     <row r="29" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="6">
-        <v>43103</v>
+        <v>37</v>
+      </c>
+      <c r="C29" s="14">
+        <v>43095</v>
       </c>
       <c r="D29" s="7">
         <f t="shared" si="0"/>
         <v>43105</v>
       </c>
       <c r="E29" s="11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F29" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G29" s="9">
-        <f t="shared" si="4"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="H29" s="10">
         <v>0</v>
@@ -3660,25 +5884,25 @@
     </row>
     <row r="30" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C30" s="6">
-        <v>43105</v>
+        <v>43103</v>
       </c>
       <c r="D30" s="7">
         <f t="shared" si="0"/>
-        <v>43110</v>
+        <v>43105</v>
       </c>
       <c r="E30" s="11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F30" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G30" s="9">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="H30" s="10">
         <v>0</v>
@@ -3686,25 +5910,25 @@
     </row>
     <row r="31" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" s="6">
+        <v>43105</v>
+      </c>
+      <c r="D31" s="7">
+        <f t="shared" si="0"/>
         <v>43110</v>
       </c>
-      <c r="D31" s="7">
-        <f t="shared" ref="D31:D32" si="9">IF(ISBLANK(E31),"",E31+C31)</f>
-        <v>43111</v>
-      </c>
       <c r="E31" s="11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F31" s="9">
-        <f t="shared" ref="F31:F32" si="10">IF(((D31)=""),"",(H31)*(D31-C31))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G31" s="9">
-        <f t="shared" ref="G31:G32" si="11">IF(F31="","",(D31-C31)-F31)</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="H31" s="10">
         <v>0</v>
@@ -3712,25 +5936,25 @@
     </row>
     <row r="32" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" s="6">
+        <v>43110</v>
+      </c>
+      <c r="D32" s="7">
+        <f t="shared" si="0"/>
         <v>43111</v>
       </c>
-      <c r="D32" s="7">
-        <f t="shared" si="9"/>
-        <v>43114</v>
-      </c>
       <c r="E32" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F32" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G32" s="9">
-        <f t="shared" si="11"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="H32" s="10">
         <v>0</v>
@@ -3738,110 +5962,127 @@
     </row>
     <row r="33" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C33" s="6">
-        <v>42979</v>
+        <v>43111</v>
       </c>
       <c r="D33" s="7">
         <f t="shared" si="0"/>
-        <v>43129</v>
+        <v>43114</v>
       </c>
       <c r="E33" s="11">
-        <v>150</v>
+        <v>3</v>
       </c>
       <c r="F33" s="9">
-        <f t="shared" si="3"/>
-        <v>7.5</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G33" s="9">
-        <f t="shared" si="4"/>
-        <v>142.5</v>
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="H33" s="10">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C34" s="6">
-        <v>43101</v>
+        <v>42979</v>
       </c>
       <c r="D34" s="7">
         <f t="shared" si="0"/>
-        <v>43131</v>
+        <v>43129</v>
       </c>
       <c r="E34" s="11">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="F34" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>7.5</v>
       </c>
       <c r="G34" s="9">
-        <f t="shared" si="4"/>
-        <v>30</v>
+        <f t="shared" si="2"/>
+        <v>142.5</v>
       </c>
       <c r="H34" s="10">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="35" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C35" s="6">
-        <v>42765</v>
+        <v>43101</v>
       </c>
       <c r="D35" s="7">
         <f t="shared" si="0"/>
+        <v>43131</v>
+      </c>
+      <c r="E35" s="11">
+        <v>30</v>
+      </c>
+      <c r="F35" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G35" s="9">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="H35" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="6">
+        <v>42765</v>
+      </c>
+      <c r="D36" s="7">
+        <f t="shared" si="0"/>
         <v>42775</v>
       </c>
-      <c r="E35" s="11">
+      <c r="E36" s="11">
         <v>10</v>
       </c>
-      <c r="F35" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G35" s="9">
-        <f t="shared" si="4"/>
+      <c r="F36" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G36" s="9">
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="H35" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="5"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="7" t="str">
+      <c r="H36" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="5"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="7" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E36" s="11"/>
-      <c r="F36" s="9" t="str">
-        <f t="shared" si="3"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="9" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G36" s="9" t="str">
-        <f t="shared" si="4"/>
+      <c r="G37" s="9" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H36" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="17"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="12"/>
+      <c r="H37" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="2:18" ht="21" x14ac:dyDescent="0.25">
       <c r="B38" s="17"/>
@@ -4088,4 +6329,1258 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:S61"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B1:H37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="2" width="52.85546875" customWidth="1"/>
+    <col min="3" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="4" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="2.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" customWidth="1"/>
+    <col min="18" max="18" width="20.140625" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" customWidth="1"/>
+    <col min="20" max="20" width="23" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" customWidth="1"/>
+    <col min="22" max="22" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:19" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="4">
+        <f>C2</f>
+        <v>42979</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+    </row>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6">
+        <v>42979</v>
+      </c>
+      <c r="D2" s="7">
+        <f t="shared" ref="D2:D37" si="0">IF(ISBLANK(E2),"",E2+C2)</f>
+        <v>42989</v>
+      </c>
+      <c r="E2" s="8">
+        <v>10</v>
+      </c>
+      <c r="F2" s="9">
+        <f t="shared" ref="F2:F37" si="1">IF(((D2)=""),"",(H2)*(D2-C2))</f>
+        <v>8</v>
+      </c>
+      <c r="G2" s="9">
+        <f t="shared" ref="G2:G37" si="2">IF(F2="","",(D2-C2)-F2)</f>
+        <v>2</v>
+      </c>
+      <c r="H2" s="10">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6">
+        <v>42982</v>
+      </c>
+      <c r="D3" s="7">
+        <f t="shared" si="0"/>
+        <v>42987</v>
+      </c>
+      <c r="E3" s="11">
+        <v>5</v>
+      </c>
+      <c r="F3" s="9">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H3" s="10">
+        <v>1</v>
+      </c>
+      <c r="J3" s="12"/>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6">
+        <v>42982</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" si="0"/>
+        <v>42992</v>
+      </c>
+      <c r="E4" s="11">
+        <v>10</v>
+      </c>
+      <c r="F4" s="9">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G4" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="10">
+        <v>1</v>
+      </c>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6">
+        <v>42992</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>43002</v>
+      </c>
+      <c r="E5" s="11">
+        <v>10</v>
+      </c>
+      <c r="F5" s="9">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G5" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="6">
+        <v>43003</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>43004</v>
+      </c>
+      <c r="E6" s="11">
+        <v>1</v>
+      </c>
+      <c r="F6" s="9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G6" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="6">
+        <v>42998</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>43018</v>
+      </c>
+      <c r="E7" s="11">
+        <v>20</v>
+      </c>
+      <c r="F7" s="9">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="6">
+        <v>43004</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>43006</v>
+      </c>
+      <c r="E8" s="11">
+        <v>2</v>
+      </c>
+      <c r="F8" s="9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G8" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="6">
+        <v>43018</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>43020</v>
+      </c>
+      <c r="E9" s="11">
+        <v>2</v>
+      </c>
+      <c r="F9" s="9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G9" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="6">
+        <v>43020</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>43025</v>
+      </c>
+      <c r="E10" s="11">
+        <v>5</v>
+      </c>
+      <c r="F10" s="9">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G10" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="6">
+        <v>43023</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
+        <v>43033</v>
+      </c>
+      <c r="E11" s="11">
+        <v>10</v>
+      </c>
+      <c r="F11" s="9">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G11" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="6">
+        <v>43026</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
+        <v>43028</v>
+      </c>
+      <c r="E12" s="11">
+        <v>2</v>
+      </c>
+      <c r="F12" s="9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G12" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="6">
+        <v>43026</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
+        <v>43029</v>
+      </c>
+      <c r="E13" s="11">
+        <v>3</v>
+      </c>
+      <c r="F13" s="9">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G13" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="6">
+        <v>43030</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="0"/>
+        <v>43040</v>
+      </c>
+      <c r="E14" s="11">
+        <v>10</v>
+      </c>
+      <c r="F14" s="9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G14" s="9">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="6">
+        <v>43033</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="0"/>
+        <v>43038</v>
+      </c>
+      <c r="E15" s="11">
+        <v>5</v>
+      </c>
+      <c r="F15" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="9">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="H15" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="6">
+        <v>43038</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" si="0"/>
+        <v>43048</v>
+      </c>
+      <c r="E16" s="11">
+        <v>10</v>
+      </c>
+      <c r="F16" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="9">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H16" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="6">
+        <v>43038</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="0"/>
+        <v>43068</v>
+      </c>
+      <c r="E17" s="11">
+        <v>30</v>
+      </c>
+      <c r="F17" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="9">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="H17" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="6">
+        <v>43049</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" si="0"/>
+        <v>43054</v>
+      </c>
+      <c r="E18" s="11">
+        <v>5</v>
+      </c>
+      <c r="F18" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="9">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="6">
+        <v>43054</v>
+      </c>
+      <c r="D19" s="7">
+        <f t="shared" si="0"/>
+        <v>43074</v>
+      </c>
+      <c r="E19" s="11">
+        <v>20</v>
+      </c>
+      <c r="F19" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="9">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="H19" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="6">
+        <v>43070</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" ref="D20" si="3">IF(ISBLANK(E20),"",E20+C20)</f>
+        <v>43080</v>
+      </c>
+      <c r="E20" s="11">
+        <v>10</v>
+      </c>
+      <c r="F20" s="9">
+        <f t="shared" ref="F20" si="4">IF(((D20)=""),"",(H20)*(D20-C20))</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="9">
+        <f t="shared" ref="G20" si="5">IF(F20="","",(D20-C20)-F20)</f>
+        <v>10</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="6">
+        <v>43070</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="0"/>
+        <v>43080</v>
+      </c>
+      <c r="E21" s="11">
+        <v>10</v>
+      </c>
+      <c r="F21" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="9">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H21" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="6">
+        <v>43080</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="0"/>
+        <v>43081</v>
+      </c>
+      <c r="E22" s="11">
+        <v>1</v>
+      </c>
+      <c r="F22" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H22" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="6">
+        <v>43081</v>
+      </c>
+      <c r="D23" s="7">
+        <f t="shared" si="0"/>
+        <v>43084</v>
+      </c>
+      <c r="E23" s="11">
+        <v>3</v>
+      </c>
+      <c r="F23" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="9">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="H23" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="6">
+        <v>43082</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" si="0"/>
+        <v>43085</v>
+      </c>
+      <c r="E24" s="15">
+        <v>3</v>
+      </c>
+      <c r="F24" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="9">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="H24" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="6">
+        <v>43083</v>
+      </c>
+      <c r="D25" s="7">
+        <f t="shared" si="0"/>
+        <v>43086</v>
+      </c>
+      <c r="E25" s="15">
+        <v>3</v>
+      </c>
+      <c r="F25" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="9">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="H25" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="14">
+        <v>43086</v>
+      </c>
+      <c r="D26" s="7">
+        <f t="shared" si="0"/>
+        <v>43088</v>
+      </c>
+      <c r="E26" s="15">
+        <v>2</v>
+      </c>
+      <c r="F26" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="9">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="H26" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="14">
+        <v>43088</v>
+      </c>
+      <c r="D27" s="7">
+        <f t="shared" si="0"/>
+        <v>43093</v>
+      </c>
+      <c r="E27" s="15">
+        <v>5</v>
+      </c>
+      <c r="F27" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="9">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="H27" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="14">
+        <v>43091</v>
+      </c>
+      <c r="D28" s="7">
+        <f t="shared" si="0"/>
+        <v>43094</v>
+      </c>
+      <c r="E28" s="11">
+        <v>3</v>
+      </c>
+      <c r="F28" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G28" s="9">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="H28" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="14">
+        <v>43095</v>
+      </c>
+      <c r="D29" s="7">
+        <f t="shared" si="0"/>
+        <v>43105</v>
+      </c>
+      <c r="E29" s="11">
+        <v>10</v>
+      </c>
+      <c r="F29" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="9">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H29" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="6">
+        <v>43103</v>
+      </c>
+      <c r="D30" s="7">
+        <f t="shared" si="0"/>
+        <v>43105</v>
+      </c>
+      <c r="E30" s="11">
+        <v>2</v>
+      </c>
+      <c r="F30" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="9">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="H30" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="6">
+        <v>43105</v>
+      </c>
+      <c r="D31" s="7">
+        <f t="shared" si="0"/>
+        <v>43110</v>
+      </c>
+      <c r="E31" s="11">
+        <v>5</v>
+      </c>
+      <c r="F31" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="9">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="H31" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="6">
+        <v>43110</v>
+      </c>
+      <c r="D32" s="7">
+        <f t="shared" si="0"/>
+        <v>43111</v>
+      </c>
+      <c r="E32" s="11">
+        <v>1</v>
+      </c>
+      <c r="F32" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H32" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="6">
+        <v>43111</v>
+      </c>
+      <c r="D33" s="7">
+        <f t="shared" si="0"/>
+        <v>43114</v>
+      </c>
+      <c r="E33" s="11">
+        <v>3</v>
+      </c>
+      <c r="F33" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="9">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="H33" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="6">
+        <v>42979</v>
+      </c>
+      <c r="D34" s="7">
+        <f t="shared" si="0"/>
+        <v>43129</v>
+      </c>
+      <c r="E34" s="11">
+        <v>150</v>
+      </c>
+      <c r="F34" s="9">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="G34" s="9">
+        <f t="shared" si="2"/>
+        <v>142.5</v>
+      </c>
+      <c r="H34" s="10">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="6">
+        <v>43101</v>
+      </c>
+      <c r="D35" s="7">
+        <f t="shared" si="0"/>
+        <v>43131</v>
+      </c>
+      <c r="E35" s="11">
+        <v>30</v>
+      </c>
+      <c r="F35" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G35" s="9">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="H35" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="6">
+        <v>42765</v>
+      </c>
+      <c r="D36" s="7">
+        <f t="shared" si="0"/>
+        <v>42775</v>
+      </c>
+      <c r="E36" s="11">
+        <v>10</v>
+      </c>
+      <c r="F36" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G36" s="9">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H36" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="5"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E37" s="11"/>
+      <c r="F37" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G37" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H37" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="17"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="12"/>
+    </row>
+    <row r="39" spans="2:18" ht="21" x14ac:dyDescent="0.25">
+      <c r="B39" s="17"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="12"/>
+      <c r="J39" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="K39" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="L39" s="23"/>
+      <c r="M39" s="23"/>
+      <c r="N39" s="23"/>
+      <c r="O39" s="23"/>
+      <c r="P39" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q39" s="24"/>
+      <c r="R39" s="24"/>
+    </row>
+    <row r="40" spans="2:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="17"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="K40" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="L40" s="25"/>
+      <c r="M40" s="25"/>
+      <c r="N40" s="25"/>
+      <c r="O40" s="25"/>
+      <c r="P40" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q40" s="25"/>
+      <c r="R40" s="25"/>
+    </row>
+    <row r="41" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="17"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+    </row>
+    <row r="42" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="17"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+    </row>
+    <row r="43" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="17"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+    </row>
+    <row r="44" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="17"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+    </row>
+    <row r="45" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="17"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+    </row>
+    <row r="46" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="17"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+    </row>
+    <row r="47" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="17"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+    </row>
+    <row r="48" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="17"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+    </row>
+    <row r="49" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="17"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+    </row>
+    <row r="50" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="17"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+    </row>
+    <row r="51" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="17"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+    </row>
+    <row r="52" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="17"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+    </row>
+    <row r="53" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="17"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+    </row>
+    <row r="54" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="17"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+    </row>
+    <row r="55" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="17"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+    </row>
+    <row r="56" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="17"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+    </row>
+    <row r="57" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="17"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+    </row>
+    <row r="58" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="17"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18"/>
+    </row>
+    <row r="59" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="17"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
+    </row>
+    <row r="60" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="17"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+    </row>
+    <row r="61" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="17"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="M1:S1"/>
+    <mergeCell ref="K39:O39"/>
+    <mergeCell ref="P39:R39"/>
+    <mergeCell ref="K40:O40"/>
+    <mergeCell ref="P40:R40"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>